<commit_message>
Cambiado nombre Skyway a 7001353, añadidas variables para funcion de formateo de tabla
</commit_message>
<xml_diff>
--- a/AI_Engine/Info/codigo_sap_clientes.xlsx
+++ b/AI_Engine/Info/codigo_sap_clientes.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proyectos\Nueva carpeta\Bot-Creacion-de-Pedidos\AI_Engine\Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD7531D-8D13-4178-B250-44E3F1D8D3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B1A00F-3D54-4D95-A8C6-1B7F8D87AFA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4190" yWindow="11060" windowWidth="10620" windowHeight="10160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8400" yWindow="3120" windowWidth="16995" windowHeight="10230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$1</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>Customer</t>
   </si>
@@ -49,21 +52,12 @@
     <t>Coffeyville Sektam</t>
   </si>
   <si>
-    <t>70004530</t>
-  </si>
-  <si>
     <t>Concentric India</t>
   </si>
   <si>
-    <t>70016983</t>
-  </si>
-  <si>
     <t>Daleo</t>
   </si>
   <si>
-    <t>70001353</t>
-  </si>
-  <si>
     <t>EMP</t>
   </si>
   <si>
@@ -82,9 +76,6 @@
     <t>Hypro</t>
   </si>
   <si>
-    <t>70017109</t>
-  </si>
-  <si>
     <t>Manheim</t>
   </si>
   <si>
@@ -94,9 +85,6 @@
     <t>PARKER</t>
   </si>
   <si>
-    <t>70017128</t>
-  </si>
-  <si>
     <t>REMAN Springfield</t>
   </si>
   <si>
@@ -112,15 +100,9 @@
     <t>Sauer-Danfoss</t>
   </si>
   <si>
-    <t>70013219</t>
-  </si>
-  <si>
     <t>Soucy</t>
   </si>
   <si>
-    <t>70018728</t>
-  </si>
-  <si>
     <t>TIG</t>
   </si>
   <si>
@@ -173,6 +155,12 @@
   </si>
   <si>
     <t>Thyssenkrupp Campo Limpo</t>
+  </si>
+  <si>
+    <t>Nombre completo</t>
+  </si>
+  <si>
+    <t>Skyway</t>
   </si>
 </sst>
 </file>
@@ -535,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,222 +543,241 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>7001353</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>70001256</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
+      <c r="B4">
+        <v>70001353</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>70004530</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>70012672</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B7">
-        <v>70017703</v>
-      </c>
-      <c r="C7" t="s">
-        <v>44</v>
+        <v>70013219</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>70001256</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
+        <v>70016983</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>70017048</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>70017078</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>70017109</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>70017128</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
+        <v>32</v>
+      </c>
+      <c r="B13">
+        <v>70017673</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" t="s">
-        <v>24</v>
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>70017703</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>70017869</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>70018728</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B17">
-        <v>70017869</v>
+        <v>70018938</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18">
-        <v>70017078</v>
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19">
-        <v>70017048</v>
-      </c>
-      <c r="C19" t="s">
-        <v>45</v>
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23">
-        <v>70018938</v>
-      </c>
-      <c r="C23" t="s">
-        <v>40</v>
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24">
-        <v>70017673</v>
+        <v>16</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C24">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
Añadido configuracion multiple por proveedor, nueva configuracion para ESP, formateo de codigo
</commit_message>
<xml_diff>
--- a/AI_Engine/Info/codigo_sap_clientes.xlsx
+++ b/AI_Engine/Info/codigo_sap_clientes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proyectos\Nueva carpeta\Bot-Creacion-de-Pedidos\AI_Engine\Info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deere-my.sharepoint.com/personal/gonzalezdiazsergio_johndeere_com/Documents/Desktop/Proyectos/Bot-Creacion-de-Pedidos/AI_Engine/Info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B1A00F-3D54-4D95-A8C6-1B7F8D87AFA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00B1A00F-3D54-4D95-A8C6-1B7F8D87AFA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8862A567-3E9C-4B78-8F68-E9336E5767F9}"/>
   <bookViews>
-    <workbookView xWindow="8400" yWindow="3120" windowWidth="16995" windowHeight="10230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2400" yWindow="9900" windowWidth="13950" windowHeight="11330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -526,7 +526,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +552,7 @@
         <v>41</v>
       </c>
       <c r="B2">
-        <v>7001353</v>
+        <v>70001353</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>

</xml_diff>